<commit_message>
Adding Manual test cases for computer DB
</commit_message>
<xml_diff>
--- a/ComputerDB Test Cases.xlsx
+++ b/ComputerDB Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgunda/automation/Netflix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD245E4-3C10-484F-B709-072E62B8E3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D88DFA-0C98-5741-86EA-77A98689E976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15460" yWindow="4040" windowWidth="36020" windowHeight="25380" xr2:uid="{E8D315CF-D9F0-F748-9EBF-9B5053144B19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
   <si>
     <t xml:space="preserve">Test Title </t>
   </si>
@@ -374,6 +374,122 @@
 4.) Cllck on the name which need to be eddited 
 5.) make some edits to the record
 6.) click on "Cancel" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete a record </t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName which need to be edited
+3.) Click on filter by name
+4.) Cllck on the name which need to be eddited 
+5.) make some edits to the record
+6.) click on "Delete this computer" button on right most corner</t>
+  </si>
+  <si>
+    <t>The record should be delted and a success message should be displayed on home page</t>
+  </si>
+  <si>
+    <t>Search a Deleted record</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName which is deleted
+3.) Click on filter by name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A message should be shown that "Nothing to display should be shown" </t>
+  </si>
+  <si>
+    <t>All valid record with search name should be displayed</t>
+  </si>
+  <si>
+    <t>Search a record with valid computer name</t>
+  </si>
+  <si>
+    <t>Search a record with prefix computer name</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName with prefix computer name
+3.) Click on filter by name</t>
+  </si>
+  <si>
+    <t>Search a record with partial computer name</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName with partial computer name
+3.) Click on filter by name</t>
+  </si>
+  <si>
+    <t>Search a record with computer name which have sepcial symboles</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName which has computer name with special symbloes
+3.) Click on filter by name</t>
+  </si>
+  <si>
+    <t>Search a record with computer name which contains sub string</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName which contains substring of name
+3.) Click on filter by name</t>
+  </si>
+  <si>
+    <t>No record should be displayed</t>
+  </si>
+  <si>
+    <t>Access home page</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) verify and validate all the element in home page</t>
+  </si>
+  <si>
+    <t>All the elements should displayed in designated places and elements should be aligned when there is a change in screen resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify all element in Edit page </t>
+  </si>
+  <si>
+    <t>Verify all element in Home page</t>
+  </si>
+  <si>
+    <t>Search a record and access Edit  page</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search a computerName which need to be edited
+3.) Click on filter by name
+4.) Cllck on the name which need to be eddited 
+5.) Validate if all the elements are displayed properly on edit page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify all element in Add page </t>
+  </si>
+  <si>
+    <t>Access Add page</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Click on add new computer
+3.) Verify all element in the screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify all the CURD operation in different browsers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install all valid browsers or have access to cloud which can provid all different browsers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.) Load URL in different browsers 
+2.) Veify all CURD operation in different browsers like, Mweb, safari, edge, chrome, firefox ,  opera etc </t>
+  </si>
+  <si>
+    <t>All the elements should displayed in designated places and elements should be aligned when there is a change in screen resolution base on different browsers</t>
   </si>
 </sst>
 </file>
@@ -750,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D17EC2-1F1D-7440-899C-6D41824228F9}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1222,62 +1338,194 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Adding few more manual records
</commit_message>
<xml_diff>
--- a/ComputerDB Test Cases.xlsx
+++ b/ComputerDB Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgunda/automation/Netflix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D88DFA-0C98-5741-86EA-77A98689E976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D70ADF-ABB7-7C40-8723-8A822E9899F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15460" yWindow="4040" windowWidth="36020" windowHeight="25380" xr2:uid="{E8D315CF-D9F0-F748-9EBF-9B5053144B19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="125">
   <si>
     <t xml:space="preserve">Test Title </t>
   </si>
@@ -490,6 +490,58 @@
   </si>
   <si>
     <t>All the elements should displayed in designated places and elements should be aligned when there is a change in screen resolution base on different browsers</t>
+  </si>
+  <si>
+    <t>Verify pagination on Home page</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Check for pagination elements at the bottom of home page
+3.) Click on next and previous buttons</t>
+  </si>
+  <si>
+    <t>Verify that all the page should be displayed and only 10 record are shown per page, and when next button is clicked subsequent 10 more records should be shown in accending order. When previousl button is access previous 10 record should be accessed</t>
+  </si>
+  <si>
+    <t>Verify end of  on Home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.) Load URL  
+2.) Check for pagination elements at the bottom of home page
+3.) Click on next untill end of home page is reached </t>
+  </si>
+  <si>
+    <t>Next button should be disabled</t>
+  </si>
+  <si>
+    <t>Verify beginning of  on Home page</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Check for pagination elements at the bottom of home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous button should be disabled when there are no more than 10 record and if the home page is at the bening of all records. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify pagenation on search value </t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search for a computer name which have less than 10 records</t>
+  </si>
+  <si>
+    <t>Next and Previous button should not be displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify pagenation on search value with more than 10 records</t>
+  </si>
+  <si>
+    <t>1.) Load URL  
+2.) Search for a computer name which have more than 10 records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next  button should not be enabled, and by clicking it should display next set of records. </t>
   </si>
 </sst>
 </file>
@@ -864,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D17EC2-1F1D-7440-899C-6D41824228F9}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="117" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1525,9 +1577,89 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>